<commit_message>
update comentarios de codigo y correlacion
</commit_message>
<xml_diff>
--- a/spearmanbitcoin.xlsx
+++ b/spearmanbitcoin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvera\Desktop\programatesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211321A8-968C-4010-A212-46782C2248D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A359EE5C-503F-4D6C-8210-05C05B9A17D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="spearmanbitcoin" sheetId="1" r:id="rId1"/>
@@ -790,9 +790,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -23042,7 +23044,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -23052,10 +23054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C09290E-8AC5-4F72-BC7D-C2342C42309E}">
-  <dimension ref="A1:AM52"/>
+  <dimension ref="A1:AM59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="Q1" sqref="Q1:AB1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25589,29 +25591,36 @@
         <v>0.43046499798098897</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D49" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D50" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D51" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:32" x14ac:dyDescent="0.25">
       <c r="D52" t="s">
         <v>88</v>
       </c>
+    </row>
+    <row r="56" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="AE56" s="2"/>
+    </row>
+    <row r="59" spans="4:32" x14ac:dyDescent="0.25">
+      <c r="AD59" s="3"/>
+      <c r="AF59" s="3"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:AM39">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"x"</formula>
     </cfRule>
     <cfRule type="colorScale" priority="2">
@@ -25635,7 +25644,7 @@
   <dimension ref="A1:AM39"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z43" sqref="Z43"/>
+      <selection activeCell="A10" activeCellId="2" sqref="G10:H1048576 G1:H8 A10:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28193,8 +28202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFA7F3E0-E953-4386-A757-C9CA2D4A40A1}">
   <dimension ref="A1:AN46"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>